<commit_message>
variable prices and extra level
</commit_message>
<xml_diff>
--- a/Perseverance/data/level1.xlsx
+++ b/Perseverance/data/level1.xlsx
@@ -544,7 +544,41 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -838,15 +872,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DP13"/>
+  <dimension ref="A1:CV13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="BU26" sqref="BU26"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="CK42" sqref="CK42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
@@ -1076,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="BY1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ1">
         <v>0</v>
@@ -1139,76 +1173,16 @@
         <v>0</v>
       </c>
       <c r="CT1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CU1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV1">
-        <v>0</v>
-      </c>
-      <c r="CW1">
-        <v>0</v>
-      </c>
-      <c r="CX1">
-        <v>0</v>
-      </c>
-      <c r="CY1">
-        <v>0</v>
-      </c>
-      <c r="CZ1">
-        <v>0</v>
-      </c>
-      <c r="DA1">
-        <v>0</v>
-      </c>
-      <c r="DB1">
-        <v>0</v>
-      </c>
-      <c r="DC1">
-        <v>0</v>
-      </c>
-      <c r="DD1">
-        <v>0</v>
-      </c>
-      <c r="DE1">
-        <v>0</v>
-      </c>
-      <c r="DF1">
-        <v>0</v>
-      </c>
-      <c r="DG1">
-        <v>0</v>
-      </c>
-      <c r="DH1">
-        <v>0</v>
-      </c>
-      <c r="DI1">
-        <v>0</v>
-      </c>
-      <c r="DJ1">
-        <v>0</v>
-      </c>
-      <c r="DK1">
-        <v>0</v>
-      </c>
-      <c r="DL1">
-        <v>1</v>
-      </c>
-      <c r="DM1">
-        <v>1</v>
-      </c>
-      <c r="DN1">
-        <v>1</v>
-      </c>
-      <c r="DO1">
-        <v>1</v>
-      </c>
-      <c r="DP1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1438,7 +1412,7 @@
         <v>1</v>
       </c>
       <c r="BY2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ2">
         <v>0</v>
@@ -1501,76 +1475,16 @@
         <v>0</v>
       </c>
       <c r="CT2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CU2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV2">
-        <v>0</v>
-      </c>
-      <c r="CW2">
-        <v>0</v>
-      </c>
-      <c r="CX2">
-        <v>0</v>
-      </c>
-      <c r="CY2">
-        <v>0</v>
-      </c>
-      <c r="CZ2">
-        <v>0</v>
-      </c>
-      <c r="DA2">
-        <v>0</v>
-      </c>
-      <c r="DB2">
-        <v>0</v>
-      </c>
-      <c r="DC2">
-        <v>0</v>
-      </c>
-      <c r="DD2">
-        <v>0</v>
-      </c>
-      <c r="DE2">
-        <v>0</v>
-      </c>
-      <c r="DF2">
-        <v>0</v>
-      </c>
-      <c r="DG2">
-        <v>0</v>
-      </c>
-      <c r="DH2">
-        <v>0</v>
-      </c>
-      <c r="DI2">
-        <v>0</v>
-      </c>
-      <c r="DJ2">
-        <v>0</v>
-      </c>
-      <c r="DK2">
-        <v>0</v>
-      </c>
-      <c r="DL2">
-        <v>1</v>
-      </c>
-      <c r="DM2">
-        <v>1</v>
-      </c>
-      <c r="DN2">
-        <v>1</v>
-      </c>
-      <c r="DO2">
-        <v>1</v>
-      </c>
-      <c r="DP2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1863,76 +1777,16 @@
         <v>0</v>
       </c>
       <c r="CT3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CU3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV3">
-        <v>0</v>
-      </c>
-      <c r="CW3">
-        <v>0</v>
-      </c>
-      <c r="CX3">
-        <v>0</v>
-      </c>
-      <c r="CY3">
-        <v>0</v>
-      </c>
-      <c r="CZ3">
-        <v>0</v>
-      </c>
-      <c r="DA3">
-        <v>0</v>
-      </c>
-      <c r="DB3">
-        <v>0</v>
-      </c>
-      <c r="DC3">
-        <v>0</v>
-      </c>
-      <c r="DD3">
-        <v>0</v>
-      </c>
-      <c r="DE3">
-        <v>0</v>
-      </c>
-      <c r="DF3">
-        <v>0</v>
-      </c>
-      <c r="DG3">
-        <v>0</v>
-      </c>
-      <c r="DH3">
-        <v>0</v>
-      </c>
-      <c r="DI3">
-        <v>0</v>
-      </c>
-      <c r="DJ3">
-        <v>0</v>
-      </c>
-      <c r="DK3">
-        <v>0</v>
-      </c>
-      <c r="DL3">
-        <v>1</v>
-      </c>
-      <c r="DM3">
-        <v>1</v>
-      </c>
-      <c r="DN3">
-        <v>1</v>
-      </c>
-      <c r="DO3">
-        <v>1</v>
-      </c>
-      <c r="DP3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2225,76 +2079,16 @@
         <v>0</v>
       </c>
       <c r="CT4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CU4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV4">
-        <v>0</v>
-      </c>
-      <c r="CW4">
-        <v>0</v>
-      </c>
-      <c r="CX4">
-        <v>0</v>
-      </c>
-      <c r="CY4">
-        <v>0</v>
-      </c>
-      <c r="CZ4">
-        <v>0</v>
-      </c>
-      <c r="DA4">
-        <v>0</v>
-      </c>
-      <c r="DB4">
-        <v>0</v>
-      </c>
-      <c r="DC4">
-        <v>0</v>
-      </c>
-      <c r="DD4">
-        <v>0</v>
-      </c>
-      <c r="DE4">
-        <v>0</v>
-      </c>
-      <c r="DF4">
-        <v>0</v>
-      </c>
-      <c r="DG4">
-        <v>0</v>
-      </c>
-      <c r="DH4">
-        <v>0</v>
-      </c>
-      <c r="DI4">
-        <v>0</v>
-      </c>
-      <c r="DJ4">
-        <v>0</v>
-      </c>
-      <c r="DK4">
-        <v>0</v>
-      </c>
-      <c r="DL4">
-        <v>1</v>
-      </c>
-      <c r="DM4">
-        <v>1</v>
-      </c>
-      <c r="DN4">
-        <v>1</v>
-      </c>
-      <c r="DO4">
-        <v>1</v>
-      </c>
-      <c r="DP4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2587,76 +2381,16 @@
         <v>0</v>
       </c>
       <c r="CT5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CU5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV5">
-        <v>0</v>
-      </c>
-      <c r="CW5">
-        <v>0</v>
-      </c>
-      <c r="CX5">
-        <v>0</v>
-      </c>
-      <c r="CY5">
-        <v>0</v>
-      </c>
-      <c r="CZ5">
-        <v>0</v>
-      </c>
-      <c r="DA5">
-        <v>0</v>
-      </c>
-      <c r="DB5">
-        <v>0</v>
-      </c>
-      <c r="DC5">
-        <v>0</v>
-      </c>
-      <c r="DD5">
-        <v>0</v>
-      </c>
-      <c r="DE5">
-        <v>0</v>
-      </c>
-      <c r="DF5">
-        <v>0</v>
-      </c>
-      <c r="DG5">
-        <v>0</v>
-      </c>
-      <c r="DH5">
-        <v>0</v>
-      </c>
-      <c r="DI5">
-        <v>0</v>
-      </c>
-      <c r="DJ5">
-        <v>0</v>
-      </c>
-      <c r="DK5">
-        <v>0</v>
-      </c>
-      <c r="DL5">
-        <v>1</v>
-      </c>
-      <c r="DM5">
-        <v>1</v>
-      </c>
-      <c r="DN5">
-        <v>1</v>
-      </c>
-      <c r="DO5">
-        <v>1</v>
-      </c>
-      <c r="DP5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2886,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="BY6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ6">
         <v>0</v>
@@ -2952,73 +2686,13 @@
         <v>0</v>
       </c>
       <c r="CU6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV6">
-        <v>0</v>
-      </c>
-      <c r="CW6">
-        <v>0</v>
-      </c>
-      <c r="CX6">
-        <v>0</v>
-      </c>
-      <c r="CY6">
-        <v>0</v>
-      </c>
-      <c r="CZ6">
-        <v>0</v>
-      </c>
-      <c r="DA6">
-        <v>0</v>
-      </c>
-      <c r="DB6">
-        <v>0</v>
-      </c>
-      <c r="DC6">
-        <v>0</v>
-      </c>
-      <c r="DD6">
-        <v>0</v>
-      </c>
-      <c r="DE6">
-        <v>0</v>
-      </c>
-      <c r="DF6">
-        <v>0</v>
-      </c>
-      <c r="DG6">
-        <v>0</v>
-      </c>
-      <c r="DH6">
-        <v>0</v>
-      </c>
-      <c r="DI6">
-        <v>0</v>
-      </c>
-      <c r="DJ6">
-        <v>0</v>
-      </c>
-      <c r="DK6">
-        <v>0</v>
-      </c>
-      <c r="DL6">
-        <v>0</v>
-      </c>
-      <c r="DM6">
-        <v>1</v>
-      </c>
-      <c r="DN6">
-        <v>1</v>
-      </c>
-      <c r="DO6">
-        <v>1</v>
-      </c>
-      <c r="DP6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -3275,7 +2949,7 @@
         <v>0</v>
       </c>
       <c r="CH7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CI7">
         <v>0</v>
@@ -3290,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="CM7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CN7">
         <v>0</v>
@@ -3308,10 +2982,10 @@
         <v>0</v>
       </c>
       <c r="CS7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CT7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CU7">
         <v>0</v>
@@ -3319,68 +2993,8 @@
       <c r="CV7">
         <v>0</v>
       </c>
-      <c r="CW7">
-        <v>0</v>
-      </c>
-      <c r="CX7">
-        <v>0</v>
-      </c>
-      <c r="CY7">
-        <v>0</v>
-      </c>
-      <c r="CZ7">
-        <v>0</v>
-      </c>
-      <c r="DA7">
-        <v>0</v>
-      </c>
-      <c r="DB7">
-        <v>0</v>
-      </c>
-      <c r="DC7">
-        <v>0</v>
-      </c>
-      <c r="DD7">
-        <v>0</v>
-      </c>
-      <c r="DE7">
-        <v>0</v>
-      </c>
-      <c r="DF7">
-        <v>0</v>
-      </c>
-      <c r="DG7">
-        <v>0</v>
-      </c>
-      <c r="DH7">
-        <v>0</v>
-      </c>
-      <c r="DI7">
-        <v>0</v>
-      </c>
-      <c r="DJ7">
-        <v>0</v>
-      </c>
-      <c r="DK7">
-        <v>0</v>
-      </c>
-      <c r="DL7">
-        <v>0</v>
-      </c>
-      <c r="DM7">
-        <v>0</v>
-      </c>
-      <c r="DN7">
-        <v>0</v>
-      </c>
-      <c r="DO7">
-        <v>0</v>
-      </c>
-      <c r="DP7">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -3622,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="CC8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CD8">
         <v>0</v>
@@ -3670,10 +3284,10 @@
         <v>0</v>
       </c>
       <c r="CS8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CT8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CU8">
         <v>0</v>
@@ -3681,68 +3295,8 @@
       <c r="CV8">
         <v>0</v>
       </c>
-      <c r="CW8">
-        <v>0</v>
-      </c>
-      <c r="CX8">
-        <v>0</v>
-      </c>
-      <c r="CY8">
-        <v>0</v>
-      </c>
-      <c r="CZ8">
-        <v>0</v>
-      </c>
-      <c r="DA8">
-        <v>0</v>
-      </c>
-      <c r="DB8">
-        <v>0</v>
-      </c>
-      <c r="DC8">
-        <v>0</v>
-      </c>
-      <c r="DD8">
-        <v>0</v>
-      </c>
-      <c r="DE8">
-        <v>0</v>
-      </c>
-      <c r="DF8">
-        <v>0</v>
-      </c>
-      <c r="DG8">
-        <v>0</v>
-      </c>
-      <c r="DH8">
-        <v>0</v>
-      </c>
-      <c r="DI8">
-        <v>0</v>
-      </c>
-      <c r="DJ8">
-        <v>0</v>
-      </c>
-      <c r="DK8">
-        <v>0</v>
-      </c>
-      <c r="DL8">
-        <v>0</v>
-      </c>
-      <c r="DM8">
-        <v>0</v>
-      </c>
-      <c r="DN8">
-        <v>0</v>
-      </c>
-      <c r="DO8">
-        <v>0</v>
-      </c>
-      <c r="DP8">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4002,109 +3556,49 @@
         <v>0</v>
       </c>
       <c r="CI9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CL9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM9">
         <v>0</v>
       </c>
       <c r="CN9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CQ9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CR9">
         <v>0</v>
       </c>
       <c r="CS9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CT9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CU9">
         <v>0</v>
       </c>
       <c r="CV9">
-        <v>1</v>
-      </c>
-      <c r="CW9">
-        <v>1</v>
-      </c>
-      <c r="CX9">
-        <v>1</v>
-      </c>
-      <c r="CY9">
-        <v>1</v>
-      </c>
-      <c r="CZ9">
-        <v>0</v>
-      </c>
-      <c r="DA9">
-        <v>1</v>
-      </c>
-      <c r="DB9">
-        <v>1</v>
-      </c>
-      <c r="DC9">
-        <v>1</v>
-      </c>
-      <c r="DD9">
-        <v>1</v>
-      </c>
-      <c r="DE9">
-        <v>0</v>
-      </c>
-      <c r="DF9">
-        <v>0</v>
-      </c>
-      <c r="DG9">
-        <v>1</v>
-      </c>
-      <c r="DH9">
-        <v>1</v>
-      </c>
-      <c r="DI9">
-        <v>1</v>
-      </c>
-      <c r="DJ9">
-        <v>1</v>
-      </c>
-      <c r="DK9">
-        <v>0</v>
-      </c>
-      <c r="DL9">
-        <v>0</v>
-      </c>
-      <c r="DM9">
-        <v>0</v>
-      </c>
-      <c r="DN9">
-        <v>0</v>
-      </c>
-      <c r="DO9">
-        <v>0</v>
-      </c>
-      <c r="DP9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
@@ -4349,16 +3843,16 @@
         <v>0</v>
       </c>
       <c r="CD10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH10">
         <v>0</v>
@@ -4373,100 +3867,40 @@
         <v>0</v>
       </c>
       <c r="CL10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CP10">
         <v>0</v>
       </c>
       <c r="CQ10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CR10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CS10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CT10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CU10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV10">
-        <v>0</v>
-      </c>
-      <c r="CW10">
-        <v>0</v>
-      </c>
-      <c r="CX10">
-        <v>0</v>
-      </c>
-      <c r="CY10">
-        <v>0</v>
-      </c>
-      <c r="CZ10">
-        <v>0</v>
-      </c>
-      <c r="DA10">
-        <v>0</v>
-      </c>
-      <c r="DB10">
-        <v>0</v>
-      </c>
-      <c r="DC10">
-        <v>0</v>
-      </c>
-      <c r="DD10">
-        <v>0</v>
-      </c>
-      <c r="DE10">
-        <v>0</v>
-      </c>
-      <c r="DF10">
-        <v>0</v>
-      </c>
-      <c r="DG10">
-        <v>0</v>
-      </c>
-      <c r="DH10">
-        <v>0</v>
-      </c>
-      <c r="DI10">
-        <v>0</v>
-      </c>
-      <c r="DJ10">
-        <v>0</v>
-      </c>
-      <c r="DK10">
-        <v>0</v>
-      </c>
-      <c r="DL10">
-        <v>0</v>
-      </c>
-      <c r="DM10">
-        <v>1</v>
-      </c>
-      <c r="DN10">
-        <v>1</v>
-      </c>
-      <c r="DO10">
-        <v>1</v>
-      </c>
-      <c r="DP10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -4696,7 +4130,7 @@
         <v>0</v>
       </c>
       <c r="BY11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ11">
         <v>1</v>
@@ -4708,7 +4142,7 @@
         <v>1</v>
       </c>
       <c r="CC11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD11">
         <v>0</v>
@@ -4717,19 +4151,19 @@
         <v>0</v>
       </c>
       <c r="CF11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK11">
         <v>0</v>
@@ -4759,76 +4193,16 @@
         <v>0</v>
       </c>
       <c r="CT11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CU11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV11">
-        <v>0</v>
-      </c>
-      <c r="CW11">
-        <v>0</v>
-      </c>
-      <c r="CX11">
-        <v>0</v>
-      </c>
-      <c r="CY11">
-        <v>0</v>
-      </c>
-      <c r="CZ11">
-        <v>0</v>
-      </c>
-      <c r="DA11">
-        <v>0</v>
-      </c>
-      <c r="DB11">
-        <v>0</v>
-      </c>
-      <c r="DC11">
-        <v>0</v>
-      </c>
-      <c r="DD11">
-        <v>0</v>
-      </c>
-      <c r="DE11">
-        <v>0</v>
-      </c>
-      <c r="DF11">
-        <v>0</v>
-      </c>
-      <c r="DG11">
-        <v>0</v>
-      </c>
-      <c r="DH11">
-        <v>0</v>
-      </c>
-      <c r="DI11">
-        <v>0</v>
-      </c>
-      <c r="DJ11">
-        <v>0</v>
-      </c>
-      <c r="DK11">
-        <v>0</v>
-      </c>
-      <c r="DL11">
-        <v>1</v>
-      </c>
-      <c r="DM11">
-        <v>1</v>
-      </c>
-      <c r="DN11">
-        <v>1</v>
-      </c>
-      <c r="DO11">
-        <v>1</v>
-      </c>
-      <c r="DP11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
@@ -5055,7 +4429,7 @@
         <v>1</v>
       </c>
       <c r="BX12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY12">
         <v>0</v>
@@ -5121,76 +4495,16 @@
         <v>0</v>
       </c>
       <c r="CT12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CU12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV12">
-        <v>0</v>
-      </c>
-      <c r="CW12">
-        <v>0</v>
-      </c>
-      <c r="CX12">
-        <v>0</v>
-      </c>
-      <c r="CY12">
-        <v>0</v>
-      </c>
-      <c r="CZ12">
-        <v>0</v>
-      </c>
-      <c r="DA12">
-        <v>0</v>
-      </c>
-      <c r="DB12">
-        <v>0</v>
-      </c>
-      <c r="DC12">
-        <v>0</v>
-      </c>
-      <c r="DD12">
-        <v>0</v>
-      </c>
-      <c r="DE12">
-        <v>0</v>
-      </c>
-      <c r="DF12">
-        <v>0</v>
-      </c>
-      <c r="DG12">
-        <v>0</v>
-      </c>
-      <c r="DH12">
-        <v>0</v>
-      </c>
-      <c r="DI12">
-        <v>0</v>
-      </c>
-      <c r="DJ12">
-        <v>0</v>
-      </c>
-      <c r="DK12">
-        <v>0</v>
-      </c>
-      <c r="DL12">
-        <v>1</v>
-      </c>
-      <c r="DM12">
-        <v>1</v>
-      </c>
-      <c r="DN12">
-        <v>1</v>
-      </c>
-      <c r="DO12">
-        <v>1</v>
-      </c>
-      <c r="DP12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:120" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:100" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -5417,7 +4731,7 @@
         <v>1</v>
       </c>
       <c r="BX13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY13">
         <v>0</v>
@@ -5483,82 +4797,22 @@
         <v>0</v>
       </c>
       <c r="CT13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CU13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CV13">
-        <v>0</v>
-      </c>
-      <c r="CW13">
-        <v>0</v>
-      </c>
-      <c r="CX13">
-        <v>0</v>
-      </c>
-      <c r="CY13">
-        <v>0</v>
-      </c>
-      <c r="CZ13">
-        <v>0</v>
-      </c>
-      <c r="DA13">
-        <v>0</v>
-      </c>
-      <c r="DB13">
-        <v>0</v>
-      </c>
-      <c r="DC13">
-        <v>0</v>
-      </c>
-      <c r="DD13">
-        <v>0</v>
-      </c>
-      <c r="DE13">
-        <v>0</v>
-      </c>
-      <c r="DF13">
-        <v>0</v>
-      </c>
-      <c r="DG13">
-        <v>0</v>
-      </c>
-      <c r="DH13">
-        <v>0</v>
-      </c>
-      <c r="DI13">
-        <v>0</v>
-      </c>
-      <c r="DJ13">
-        <v>0</v>
-      </c>
-      <c r="DK13">
-        <v>0</v>
-      </c>
-      <c r="DL13">
-        <v>1</v>
-      </c>
-      <c r="DM13">
-        <v>1</v>
-      </c>
-      <c r="DN13">
-        <v>1</v>
-      </c>
-      <c r="DO13">
-        <v>1</v>
-      </c>
-      <c r="DP13">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:FD13">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="DP15 CW15 DO1:FD13 DE1:DE13 A1:CV13">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>